<commit_message>
updated with new datapoints
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ticket generation platform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\Ticket_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE47746-817F-4F8D-AD3F-CB826A6E40AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A25780-2851-431A-AECC-256EE6683861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>UserID</t>
   </si>
@@ -33,10 +33,22 @@
     <t>Password</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>user2</t>
+    <t>u1</t>
+  </si>
+  <si>
+    <t>u2</t>
+  </si>
+  <si>
+    <t>u3</t>
+  </si>
+  <si>
+    <t>u4</t>
+  </si>
+  <si>
+    <t>u5</t>
+  </si>
+  <si>
+    <t>u6</t>
   </si>
 </sst>
 </file>
@@ -354,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -375,7 +387,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1111</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -383,7 +395,39 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2222</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>